<commit_message>
Finish the digital memory palace excel
</commit_message>
<xml_diff>
--- a/数字宫殿/0-99DigitalMemoryPalace.xlsx
+++ b/数字宫殿/0-99DigitalMemoryPalace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Github\MemoryPalace\数字宫殿\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51D7F25-C582-41D5-B46B-9D3A46CC83F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A867B94-1327-4939-BA43-92A5ACE5A857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="1041">
   <si>
     <t>自行车</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2348,6 +2348,1845 @@
   </si>
   <si>
     <t>水草</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作业牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路障</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>快递车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角窗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安全帽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铲子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土坑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>液压器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轮胎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红蘑菇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三叉戟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洗衣板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烟筒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>袁芳天窗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阳台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树叶凳子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小门口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>细铁丝网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炕桌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉璧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白灯笼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>象牙木雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞天菩萨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际象棋烛台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>官员乌纱帽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>倒挂金钩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌纱帽皇上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树皮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>武士之剑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>净瓶形门洞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金条长方形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗笠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桌子侧面板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>佛头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镂空瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>象盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁索灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电线杆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火车头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挡板红色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞭望塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小黄桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢筋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>墙角自行车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸管</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>漏斗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火炬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牢笼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>眼睛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瓶盖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>座位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>破铁皮桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大炮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鲨鱼头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>船舵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>箭袋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炸药包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地道口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火炉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>围棋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神木玉鼎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁拐李石雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒樽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猪娃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玉印</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大肚佛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床板栅格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孔雀尾巴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笔洗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土著人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑墙壁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电话亭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水坑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桩子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桌子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猪头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土地雷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿色小乌龟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>莲莲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扣子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜板菜刀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菠萝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>椰子笑脸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攀爬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消防灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推土机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑梯城堡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>翻斗车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄台阶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矮桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝台阶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狮子绣球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盘龙柱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁栅栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石鼓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葫芦镂空砖雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房檐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石球红花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙隐寺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧门房间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花坛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>佛堂空间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香山</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞檐走壁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>书报亭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料袋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香柱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香灰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炉脚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄裙子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向日葵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸳鸯石膏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木舟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上吊树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玄武岩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>藤编大蓊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螺丝尖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螺丝帽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>藤编桌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锣鼓擂台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牌坊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4个玉柱子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>舞台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火刑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暗河空间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石雕龙小门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文具盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨头烟灰盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邪恶母象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑白觉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>带土面具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小内裤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电脑包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遥控器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀人漏斗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水管</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枯树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>入户门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>门灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扁担</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洗衣盆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸡窝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿漆板凳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葡萄酒酒柜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高尔基石像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树洞黄花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变态鸟笼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>福娃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金奖杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗族妹子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵马俑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>废水桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>八卦阴阳伞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子台历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>货架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿毛鬼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条幅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坐垫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>令牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵蛋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白金独角兽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>藤蔓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瀑布</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石头独角</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小鸟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>独木桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QL字样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尾翼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跑道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塔楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拖车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登机仓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>货物入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发动机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奶茶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保龄球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彩虹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>象鼻滑梯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木马</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>袋子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放大镜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大黄鸭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猪皮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红色灯笼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜山</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烟叶帆船</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南瓜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青椒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌贼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荔枝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牡蛎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灶炕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骑士铠甲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青色器材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人像机关砖雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锥形瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>垃圾箱骷髅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地砖拼花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开裂石阶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石斧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>软包塑料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直升飞机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>珠算盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吊灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>靠椅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红色大象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩具汽车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>断墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>212吉普车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>犀牛角</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>犀牛屁股</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天鹅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>池边</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干裂水坑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌鸦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电厂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷达</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兵营</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主基地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导弹车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作战指挥中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>油井</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>筒灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>镇纸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝色青蛙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无字天书</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>砚台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笔架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>画轴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>条形栅格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽屉铜拉手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鸟嘴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热气球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>肥仔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汽艇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狗嘴舌头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拐杖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爪子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>叶子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红土</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>草地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金牛头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男人石雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水枪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>松树三角形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圆珠笔建筑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巴黎塔尖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塔身</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桥头马</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白衣女孩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>射灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注射器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>话筒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>墙纸夹缝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心珍珠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫色帽子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白色蝴蝶结</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项链首饰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绵羊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒙古包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>勒勒车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晾衣架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卷帘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木头围栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛奶桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包内空间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绳子木桩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉链</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红包石心形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干树枝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胶带</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>苁蓉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羚羊角书架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇石蛋形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扇叶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大理石盒子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桌面红宝石碗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>云龙纹摆件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>巴士解剖图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>塑料花瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>银雕花烟灰缸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛇果如意果盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫檀钵</t>
+  </si>
+  <si>
+    <t>水族箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>84路巴士</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建筑残骸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青花大缸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柱子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红漆鹰盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吊着音响</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>半个足球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇石千层饼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关公</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香炉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金如意</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三层元宝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨灰盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铜龟鹤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>茶杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>花</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木雕长龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低音炮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三脚架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双层骨灰盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跪着八路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百事可乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瓶底</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉堡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瓶口处</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火烈鸟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>薯条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼群</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空盘子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>碗面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>马灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牙具盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葫芦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洗洁精</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>壶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>植物油</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纸抽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钥匙串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小黄人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香蕉头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香蕉牙齿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香蕉果肉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大头鞋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>验钞机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香蕉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长江七号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝精灵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吊顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑柱子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘴型火炉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骷髅大地毯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皮卡丘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柴火</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白鸟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91号秋衣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>夜光杯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体操人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蚯蚓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>眼镜蛇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狗食盆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼嘴型瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连体地球仪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿拉丁神灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铅笔桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水雷蜘蛛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火箭船</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞船灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木马床</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝月亮灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男背</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>液体火箭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小岛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海鸥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>椰子树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美女马赛克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>威士忌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酷西瓜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙滩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海星</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿色条纹帆船</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树根雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插排</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒杯灯罩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>双垃圾桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一串葫芦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>颜料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登高椅子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人形木雕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大酒壶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屏风</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吊钟</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒杯灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电视高晓松</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绿毛球</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蓝色马赛克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收纳桶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金酒壶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高速公路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剪刀房子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土山</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>楼房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地铁站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蜂窝楼房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体育馆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木板桥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>干裂土地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>破烂帐篷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仙人掌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>秃鹫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>骷髅铁链</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>头骨断角</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旧旗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>门口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乱石堆墓碑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>藏羹剩饭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>品酒架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>弧形接待台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扇形桌子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玻璃幕墙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旋转门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>窄弧形水池</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喷泉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵宾区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吧台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1个洞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音响</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玻璃柜子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>台湾99神功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电视柜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>似玉猪龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栅格吊顶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反光窗帘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁柱立体音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胖脸佛</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2675,8 +4514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4657,6 +6496,36 @@
       <c r="B53" t="s">
         <v>58</v>
       </c>
+      <c r="C53" t="s">
+        <v>581</v>
+      </c>
+      <c r="D53" t="s">
+        <v>582</v>
+      </c>
+      <c r="E53" t="s">
+        <v>583</v>
+      </c>
+      <c r="F53" t="s">
+        <v>584</v>
+      </c>
+      <c r="G53" t="s">
+        <v>585</v>
+      </c>
+      <c r="H53" t="s">
+        <v>586</v>
+      </c>
+      <c r="I53" t="s">
+        <v>587</v>
+      </c>
+      <c r="J53" t="s">
+        <v>588</v>
+      </c>
+      <c r="K53" t="s">
+        <v>589</v>
+      </c>
+      <c r="L53" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -4665,6 +6534,36 @@
       <c r="B54" t="s">
         <v>59</v>
       </c>
+      <c r="C54" t="s">
+        <v>591</v>
+      </c>
+      <c r="D54" t="s">
+        <v>592</v>
+      </c>
+      <c r="E54" t="s">
+        <v>593</v>
+      </c>
+      <c r="F54" t="s">
+        <v>594</v>
+      </c>
+      <c r="G54" t="s">
+        <v>595</v>
+      </c>
+      <c r="H54" t="s">
+        <v>596</v>
+      </c>
+      <c r="I54" t="s">
+        <v>597</v>
+      </c>
+      <c r="J54" t="s">
+        <v>598</v>
+      </c>
+      <c r="K54" t="s">
+        <v>599</v>
+      </c>
+      <c r="L54" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
@@ -4673,6 +6572,36 @@
       <c r="B55" t="s">
         <v>60</v>
       </c>
+      <c r="C55" t="s">
+        <v>601</v>
+      </c>
+      <c r="D55" t="s">
+        <v>602</v>
+      </c>
+      <c r="E55" t="s">
+        <v>603</v>
+      </c>
+      <c r="F55" t="s">
+        <v>604</v>
+      </c>
+      <c r="G55" t="s">
+        <v>605</v>
+      </c>
+      <c r="H55" t="s">
+        <v>606</v>
+      </c>
+      <c r="I55" t="s">
+        <v>607</v>
+      </c>
+      <c r="J55" t="s">
+        <v>608</v>
+      </c>
+      <c r="K55" t="s">
+        <v>609</v>
+      </c>
+      <c r="L55" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -4681,6 +6610,36 @@
       <c r="B56" t="s">
         <v>61</v>
       </c>
+      <c r="C56" t="s">
+        <v>611</v>
+      </c>
+      <c r="D56" t="s">
+        <v>612</v>
+      </c>
+      <c r="E56" t="s">
+        <v>613</v>
+      </c>
+      <c r="F56" t="s">
+        <v>614</v>
+      </c>
+      <c r="G56" t="s">
+        <v>615</v>
+      </c>
+      <c r="H56" t="s">
+        <v>616</v>
+      </c>
+      <c r="I56" t="s">
+        <v>617</v>
+      </c>
+      <c r="J56" t="s">
+        <v>618</v>
+      </c>
+      <c r="K56" t="s">
+        <v>619</v>
+      </c>
+      <c r="L56" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -4689,6 +6648,36 @@
       <c r="B57" t="s">
         <v>62</v>
       </c>
+      <c r="C57" t="s">
+        <v>621</v>
+      </c>
+      <c r="D57" t="s">
+        <v>622</v>
+      </c>
+      <c r="E57" t="s">
+        <v>595</v>
+      </c>
+      <c r="F57" t="s">
+        <v>623</v>
+      </c>
+      <c r="G57" t="s">
+        <v>624</v>
+      </c>
+      <c r="H57" t="s">
+        <v>625</v>
+      </c>
+      <c r="I57" t="s">
+        <v>626</v>
+      </c>
+      <c r="J57" t="s">
+        <v>627</v>
+      </c>
+      <c r="K57" t="s">
+        <v>628</v>
+      </c>
+      <c r="L57" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -4697,6 +6686,36 @@
       <c r="B58" t="s">
         <v>63</v>
       </c>
+      <c r="C58" t="s">
+        <v>630</v>
+      </c>
+      <c r="D58" t="s">
+        <v>631</v>
+      </c>
+      <c r="E58" t="s">
+        <v>238</v>
+      </c>
+      <c r="F58" t="s">
+        <v>632</v>
+      </c>
+      <c r="G58" t="s">
+        <v>633</v>
+      </c>
+      <c r="H58" t="s">
+        <v>634</v>
+      </c>
+      <c r="I58" t="s">
+        <v>635</v>
+      </c>
+      <c r="J58" t="s">
+        <v>636</v>
+      </c>
+      <c r="K58" t="s">
+        <v>637</v>
+      </c>
+      <c r="L58" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -4705,6 +6724,36 @@
       <c r="B59" t="s">
         <v>64</v>
       </c>
+      <c r="C59" t="s">
+        <v>639</v>
+      </c>
+      <c r="D59" t="s">
+        <v>640</v>
+      </c>
+      <c r="E59" t="s">
+        <v>641</v>
+      </c>
+      <c r="F59" t="s">
+        <v>642</v>
+      </c>
+      <c r="G59" t="s">
+        <v>643</v>
+      </c>
+      <c r="H59" t="s">
+        <v>644</v>
+      </c>
+      <c r="I59" t="s">
+        <v>645</v>
+      </c>
+      <c r="J59" t="s">
+        <v>646</v>
+      </c>
+      <c r="K59" t="s">
+        <v>647</v>
+      </c>
+      <c r="L59" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -4713,6 +6762,36 @@
       <c r="B60" t="s">
         <v>65</v>
       </c>
+      <c r="C60" t="s">
+        <v>649</v>
+      </c>
+      <c r="D60" t="s">
+        <v>650</v>
+      </c>
+      <c r="E60" t="s">
+        <v>651</v>
+      </c>
+      <c r="F60" t="s">
+        <v>652</v>
+      </c>
+      <c r="G60" t="s">
+        <v>653</v>
+      </c>
+      <c r="H60" t="s">
+        <v>654</v>
+      </c>
+      <c r="I60" t="s">
+        <v>655</v>
+      </c>
+      <c r="J60" t="s">
+        <v>656</v>
+      </c>
+      <c r="K60" t="s">
+        <v>657</v>
+      </c>
+      <c r="L60" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -4721,6 +6800,36 @@
       <c r="B61" t="s">
         <v>66</v>
       </c>
+      <c r="C61" t="s">
+        <v>659</v>
+      </c>
+      <c r="D61" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" t="s">
+        <v>660</v>
+      </c>
+      <c r="F61" t="s">
+        <v>661</v>
+      </c>
+      <c r="G61" t="s">
+        <v>589</v>
+      </c>
+      <c r="H61" t="s">
+        <v>662</v>
+      </c>
+      <c r="I61" t="s">
+        <v>663</v>
+      </c>
+      <c r="J61" t="s">
+        <v>664</v>
+      </c>
+      <c r="K61" t="s">
+        <v>665</v>
+      </c>
+      <c r="L61" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -4729,6 +6838,36 @@
       <c r="B62" t="s">
         <v>67</v>
       </c>
+      <c r="C62" t="s">
+        <v>667</v>
+      </c>
+      <c r="D62" t="s">
+        <v>668</v>
+      </c>
+      <c r="E62" t="s">
+        <v>669</v>
+      </c>
+      <c r="F62" t="s">
+        <v>670</v>
+      </c>
+      <c r="G62" t="s">
+        <v>671</v>
+      </c>
+      <c r="H62" t="s">
+        <v>672</v>
+      </c>
+      <c r="I62" t="s">
+        <v>673</v>
+      </c>
+      <c r="J62" t="s">
+        <v>67</v>
+      </c>
+      <c r="K62" t="s">
+        <v>674</v>
+      </c>
+      <c r="L62" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -4737,6 +6876,36 @@
       <c r="B63" t="s">
         <v>68</v>
       </c>
+      <c r="C63" t="s">
+        <v>676</v>
+      </c>
+      <c r="D63" t="s">
+        <v>677</v>
+      </c>
+      <c r="E63" t="s">
+        <v>678</v>
+      </c>
+      <c r="F63" t="s">
+        <v>679</v>
+      </c>
+      <c r="G63" t="s">
+        <v>680</v>
+      </c>
+      <c r="H63" t="s">
+        <v>681</v>
+      </c>
+      <c r="I63" t="s">
+        <v>682</v>
+      </c>
+      <c r="J63" t="s">
+        <v>683</v>
+      </c>
+      <c r="K63" t="s">
+        <v>684</v>
+      </c>
+      <c r="L63" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -4745,301 +6914,1441 @@
       <c r="B64" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>686</v>
+      </c>
+      <c r="D64" t="s">
+        <v>687</v>
+      </c>
+      <c r="E64" t="s">
+        <v>688</v>
+      </c>
+      <c r="F64" t="s">
+        <v>689</v>
+      </c>
+      <c r="G64" t="s">
+        <v>690</v>
+      </c>
+      <c r="H64" t="s">
+        <v>691</v>
+      </c>
+      <c r="I64" t="s">
+        <v>692</v>
+      </c>
+      <c r="J64" t="s">
+        <v>693</v>
+      </c>
+      <c r="K64" t="s">
+        <v>694</v>
+      </c>
+      <c r="L64" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>696</v>
+      </c>
+      <c r="D65" t="s">
+        <v>697</v>
+      </c>
+      <c r="E65" t="s">
+        <v>698</v>
+      </c>
+      <c r="F65" t="s">
+        <v>699</v>
+      </c>
+      <c r="G65" t="s">
+        <v>700</v>
+      </c>
+      <c r="H65" t="s">
+        <v>126</v>
+      </c>
+      <c r="I65" t="s">
+        <v>701</v>
+      </c>
+      <c r="J65" t="s">
+        <v>702</v>
+      </c>
+      <c r="K65" t="s">
+        <v>703</v>
+      </c>
+      <c r="L65" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>705</v>
+      </c>
+      <c r="D66" t="s">
+        <v>706</v>
+      </c>
+      <c r="E66" t="s">
+        <v>707</v>
+      </c>
+      <c r="F66" t="s">
+        <v>708</v>
+      </c>
+      <c r="G66" t="s">
+        <v>709</v>
+      </c>
+      <c r="H66" t="s">
+        <v>710</v>
+      </c>
+      <c r="I66" t="s">
+        <v>711</v>
+      </c>
+      <c r="J66" t="s">
+        <v>712</v>
+      </c>
+      <c r="K66" t="s">
+        <v>713</v>
+      </c>
+      <c r="L66" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>715</v>
+      </c>
+      <c r="D67" t="s">
+        <v>716</v>
+      </c>
+      <c r="E67" t="s">
+        <v>717</v>
+      </c>
+      <c r="F67" t="s">
+        <v>718</v>
+      </c>
+      <c r="G67" t="s">
+        <v>719</v>
+      </c>
+      <c r="H67" t="s">
+        <v>720</v>
+      </c>
+      <c r="I67" t="s">
+        <v>721</v>
+      </c>
+      <c r="J67" t="s">
+        <v>722</v>
+      </c>
+      <c r="K67" t="s">
+        <v>723</v>
+      </c>
+      <c r="L67" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>725</v>
+      </c>
+      <c r="D68" t="s">
+        <v>726</v>
+      </c>
+      <c r="E68" t="s">
+        <v>727</v>
+      </c>
+      <c r="F68" t="s">
+        <v>728</v>
+      </c>
+      <c r="G68" t="s">
+        <v>73</v>
+      </c>
+      <c r="H68" t="s">
+        <v>729</v>
+      </c>
+      <c r="I68" t="s">
+        <v>730</v>
+      </c>
+      <c r="J68" t="s">
+        <v>731</v>
+      </c>
+      <c r="K68" t="s">
+        <v>732</v>
+      </c>
+      <c r="L68" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>734</v>
+      </c>
+      <c r="D69" t="s">
+        <v>735</v>
+      </c>
+      <c r="E69" t="s">
+        <v>736</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1</v>
+      </c>
+      <c r="G69" t="s">
+        <v>737</v>
+      </c>
+      <c r="H69" t="s">
+        <v>738</v>
+      </c>
+      <c r="I69" t="s">
+        <v>739</v>
+      </c>
+      <c r="J69" t="s">
+        <v>740</v>
+      </c>
+      <c r="K69" t="s">
+        <v>741</v>
+      </c>
+      <c r="L69" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>743</v>
+      </c>
+      <c r="D70" t="s">
+        <v>744</v>
+      </c>
+      <c r="E70" t="s">
+        <v>745</v>
+      </c>
+      <c r="F70" t="s">
+        <v>746</v>
+      </c>
+      <c r="G70" t="s">
+        <v>747</v>
+      </c>
+      <c r="H70" t="s">
+        <v>748</v>
+      </c>
+      <c r="I70" t="s">
+        <v>749</v>
+      </c>
+      <c r="J70" t="s">
+        <v>75</v>
+      </c>
+      <c r="K70" t="s">
+        <v>750</v>
+      </c>
+      <c r="L70" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>752</v>
+      </c>
+      <c r="D71" t="s">
+        <v>753</v>
+      </c>
+      <c r="E71" t="s">
+        <v>754</v>
+      </c>
+      <c r="F71" t="s">
+        <v>755</v>
+      </c>
+      <c r="G71" t="s">
+        <v>756</v>
+      </c>
+      <c r="H71" t="s">
+        <v>757</v>
+      </c>
+      <c r="I71" t="s">
+        <v>758</v>
+      </c>
+      <c r="J71" t="s">
+        <v>759</v>
+      </c>
+      <c r="K71" t="s">
+        <v>760</v>
+      </c>
+      <c r="L71" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>762</v>
+      </c>
+      <c r="D72" t="s">
+        <v>763</v>
+      </c>
+      <c r="E72" t="s">
+        <v>764</v>
+      </c>
+      <c r="F72" t="s">
+        <v>765</v>
+      </c>
+      <c r="G72" t="s">
+        <v>766</v>
+      </c>
+      <c r="H72" t="s">
+        <v>767</v>
+      </c>
+      <c r="I72" t="s">
+        <v>768</v>
+      </c>
+      <c r="J72" t="s">
+        <v>769</v>
+      </c>
+      <c r="K72" t="s">
+        <v>770</v>
+      </c>
+      <c r="L72" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" t="s">
+        <v>772</v>
+      </c>
+      <c r="E73" t="s">
+        <v>773</v>
+      </c>
+      <c r="F73" t="s">
+        <v>774</v>
+      </c>
+      <c r="G73" t="s">
+        <v>775</v>
+      </c>
+      <c r="H73" t="s">
+        <v>776</v>
+      </c>
+      <c r="I73" t="s">
+        <v>777</v>
+      </c>
+      <c r="J73" t="s">
+        <v>778</v>
+      </c>
+      <c r="K73" t="s">
+        <v>779</v>
+      </c>
+      <c r="L73" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>781</v>
+      </c>
+      <c r="D74" t="s">
+        <v>782</v>
+      </c>
+      <c r="E74" t="s">
+        <v>783</v>
+      </c>
+      <c r="F74" t="s">
+        <v>784</v>
+      </c>
+      <c r="G74" t="s">
+        <v>785</v>
+      </c>
+      <c r="H74" t="s">
+        <v>786</v>
+      </c>
+      <c r="I74" t="s">
+        <v>787</v>
+      </c>
+      <c r="J74" t="s">
+        <v>788</v>
+      </c>
+      <c r="K74" t="s">
+        <v>789</v>
+      </c>
+      <c r="L74" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>791</v>
+      </c>
+      <c r="D75" t="s">
+        <v>792</v>
+      </c>
+      <c r="E75" t="s">
+        <v>793</v>
+      </c>
+      <c r="F75" t="s">
+        <v>794</v>
+      </c>
+      <c r="G75" t="s">
+        <v>795</v>
+      </c>
+      <c r="H75" t="s">
+        <v>796</v>
+      </c>
+      <c r="I75" t="s">
+        <v>797</v>
+      </c>
+      <c r="J75" t="s">
+        <v>798</v>
+      </c>
+      <c r="K75" t="s">
+        <v>799</v>
+      </c>
+      <c r="L75" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>801</v>
+      </c>
+      <c r="D76" t="s">
+        <v>802</v>
+      </c>
+      <c r="E76" t="s">
+        <v>803</v>
+      </c>
+      <c r="F76" t="s">
+        <v>804</v>
+      </c>
+      <c r="G76" t="s">
+        <v>805</v>
+      </c>
+      <c r="H76" t="s">
+        <v>806</v>
+      </c>
+      <c r="I76" t="s">
+        <v>807</v>
+      </c>
+      <c r="J76" t="s">
+        <v>808</v>
+      </c>
+      <c r="K76" t="s">
+        <v>809</v>
+      </c>
+      <c r="L76" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>811</v>
+      </c>
+      <c r="D77" t="s">
+        <v>137</v>
+      </c>
+      <c r="E77" t="s">
+        <v>812</v>
+      </c>
+      <c r="F77" t="s">
+        <v>813</v>
+      </c>
+      <c r="G77" t="s">
+        <v>814</v>
+      </c>
+      <c r="H77" t="s">
+        <v>815</v>
+      </c>
+      <c r="I77" t="s">
+        <v>816</v>
+      </c>
+      <c r="J77" t="s">
+        <v>817</v>
+      </c>
+      <c r="K77" t="s">
+        <v>385</v>
+      </c>
+      <c r="L77" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>819</v>
+      </c>
+      <c r="D78" t="s">
+        <v>820</v>
+      </c>
+      <c r="E78" t="s">
+        <v>821</v>
+      </c>
+      <c r="F78" t="s">
+        <v>822</v>
+      </c>
+      <c r="G78" t="s">
+        <v>823</v>
+      </c>
+      <c r="H78" t="s">
+        <v>824</v>
+      </c>
+      <c r="I78" t="s">
+        <v>825</v>
+      </c>
+      <c r="J78" t="s">
+        <v>826</v>
+      </c>
+      <c r="K78" t="s">
+        <v>827</v>
+      </c>
+      <c r="L78" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>829</v>
+      </c>
+      <c r="D79" t="s">
+        <v>830</v>
+      </c>
+      <c r="E79" t="s">
+        <v>831</v>
+      </c>
+      <c r="F79" t="s">
+        <v>832</v>
+      </c>
+      <c r="G79" t="s">
+        <v>833</v>
+      </c>
+      <c r="H79" t="s">
+        <v>834</v>
+      </c>
+      <c r="I79" t="s">
+        <v>412</v>
+      </c>
+      <c r="J79" t="s">
+        <v>835</v>
+      </c>
+      <c r="K79" t="s">
+        <v>836</v>
+      </c>
+      <c r="L79" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>85</v>
+      </c>
+      <c r="D80" t="s">
+        <v>838</v>
+      </c>
+      <c r="E80" t="s">
+        <v>839</v>
+      </c>
+      <c r="F80" t="s">
+        <v>840</v>
+      </c>
+      <c r="G80" t="s">
+        <v>841</v>
+      </c>
+      <c r="H80" t="s">
+        <v>842</v>
+      </c>
+      <c r="I80" t="s">
+        <v>843</v>
+      </c>
+      <c r="J80" t="s">
+        <v>844</v>
+      </c>
+      <c r="K80" t="s">
+        <v>845</v>
+      </c>
+      <c r="L80" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>847</v>
+      </c>
+      <c r="D81" t="s">
+        <v>848</v>
+      </c>
+      <c r="E81" t="s">
+        <v>849</v>
+      </c>
+      <c r="F81" t="s">
+        <v>734</v>
+      </c>
+      <c r="G81" t="s">
+        <v>86</v>
+      </c>
+      <c r="H81" t="s">
+        <v>850</v>
+      </c>
+      <c r="I81" t="s">
+        <v>851</v>
+      </c>
+      <c r="J81" t="s">
+        <v>852</v>
+      </c>
+      <c r="K81" t="s">
+        <v>853</v>
+      </c>
+      <c r="L81" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>855</v>
+      </c>
+      <c r="D82" t="s">
+        <v>856</v>
+      </c>
+      <c r="E82" t="s">
+        <v>857</v>
+      </c>
+      <c r="F82" t="s">
+        <v>858</v>
+      </c>
+      <c r="G82" t="s">
+        <v>859</v>
+      </c>
+      <c r="H82" t="s">
+        <v>860</v>
+      </c>
+      <c r="I82" t="s">
+        <v>861</v>
+      </c>
+      <c r="J82" t="s">
+        <v>862</v>
+      </c>
+      <c r="K82" t="s">
+        <v>863</v>
+      </c>
+      <c r="L82" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>865</v>
+      </c>
+      <c r="D83" t="s">
+        <v>866</v>
+      </c>
+      <c r="E83" t="s">
+        <v>867</v>
+      </c>
+      <c r="F83" t="s">
+        <v>868</v>
+      </c>
+      <c r="G83" t="s">
+        <v>869</v>
+      </c>
+      <c r="H83" t="s">
+        <v>870</v>
+      </c>
+      <c r="I83" t="s">
+        <v>787</v>
+      </c>
+      <c r="J83" t="s">
+        <v>871</v>
+      </c>
+      <c r="K83" t="s">
+        <v>872</v>
+      </c>
+      <c r="L83" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>89</v>
+      </c>
+      <c r="D84" t="s">
+        <v>874</v>
+      </c>
+      <c r="E84" t="s">
+        <v>875</v>
+      </c>
+      <c r="F84" t="s">
+        <v>876</v>
+      </c>
+      <c r="G84" t="s">
+        <v>877</v>
+      </c>
+      <c r="H84" t="s">
+        <v>878</v>
+      </c>
+      <c r="I84" t="s">
+        <v>879</v>
+      </c>
+      <c r="J84" t="s">
+        <v>880</v>
+      </c>
+      <c r="K84" t="s">
+        <v>881</v>
+      </c>
+      <c r="L84" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>883</v>
+      </c>
+      <c r="D85" t="s">
+        <v>884</v>
+      </c>
+      <c r="E85" t="s">
+        <v>885</v>
+      </c>
+      <c r="F85" t="s">
+        <v>886</v>
+      </c>
+      <c r="G85" t="s">
+        <v>90</v>
+      </c>
+      <c r="H85" t="s">
+        <v>887</v>
+      </c>
+      <c r="I85" t="s">
+        <v>888</v>
+      </c>
+      <c r="J85" t="s">
+        <v>889</v>
+      </c>
+      <c r="K85" t="s">
+        <v>890</v>
+      </c>
+      <c r="L85" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>892</v>
+      </c>
+      <c r="D86" t="s">
+        <v>893</v>
+      </c>
+      <c r="E86" t="s">
+        <v>894</v>
+      </c>
+      <c r="F86" t="s">
+        <v>895</v>
+      </c>
+      <c r="G86" t="s">
+        <v>896</v>
+      </c>
+      <c r="H86" t="s">
+        <v>897</v>
+      </c>
+      <c r="I86" t="s">
+        <v>898</v>
+      </c>
+      <c r="J86" t="s">
+        <v>899</v>
+      </c>
+      <c r="K86" t="s">
+        <v>900</v>
+      </c>
+      <c r="L86" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>902</v>
+      </c>
+      <c r="D87" t="s">
+        <v>903</v>
+      </c>
+      <c r="E87" t="s">
+        <v>904</v>
+      </c>
+      <c r="F87" t="s">
+        <v>905</v>
+      </c>
+      <c r="G87" t="s">
+        <v>906</v>
+      </c>
+      <c r="H87" t="s">
+        <v>907</v>
+      </c>
+      <c r="I87" t="s">
+        <v>908</v>
+      </c>
+      <c r="J87" t="s">
+        <v>909</v>
+      </c>
+      <c r="K87" t="s">
+        <v>910</v>
+      </c>
+      <c r="L87" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>912</v>
+      </c>
+      <c r="D88" t="s">
+        <v>913</v>
+      </c>
+      <c r="E88" t="s">
+        <v>914</v>
+      </c>
+      <c r="F88" t="s">
+        <v>915</v>
+      </c>
+      <c r="G88" t="s">
+        <v>916</v>
+      </c>
+      <c r="H88" t="s">
+        <v>917</v>
+      </c>
+      <c r="I88" t="s">
+        <v>918</v>
+      </c>
+      <c r="J88" t="s">
+        <v>919</v>
+      </c>
+      <c r="K88" t="s">
+        <v>920</v>
+      </c>
+      <c r="L88" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>922</v>
+      </c>
+      <c r="D89" t="s">
+        <v>923</v>
+      </c>
+      <c r="E89" t="s">
+        <v>924</v>
+      </c>
+      <c r="F89" t="s">
+        <v>925</v>
+      </c>
+      <c r="G89" t="s">
+        <v>926</v>
+      </c>
+      <c r="H89" t="s">
+        <v>927</v>
+      </c>
+      <c r="I89" t="s">
+        <v>94</v>
+      </c>
+      <c r="J89" t="s">
+        <v>928</v>
+      </c>
+      <c r="K89" t="s">
+        <v>929</v>
+      </c>
+      <c r="L89" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>174</v>
+      </c>
+      <c r="D90" t="s">
+        <v>931</v>
+      </c>
+      <c r="E90" t="s">
+        <v>932</v>
+      </c>
+      <c r="F90" t="s">
+        <v>933</v>
+      </c>
+      <c r="G90" t="s">
+        <v>934</v>
+      </c>
+      <c r="H90" t="s">
+        <v>935</v>
+      </c>
+      <c r="I90" t="s">
+        <v>936</v>
+      </c>
+      <c r="J90" t="s">
+        <v>937</v>
+      </c>
+      <c r="K90" t="s">
+        <v>938</v>
+      </c>
+      <c r="L90" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>940</v>
+      </c>
+      <c r="D91" t="s">
+        <v>941</v>
+      </c>
+      <c r="E91" t="s">
+        <v>942</v>
+      </c>
+      <c r="F91" t="s">
+        <v>943</v>
+      </c>
+      <c r="G91" t="s">
+        <v>944</v>
+      </c>
+      <c r="H91" t="s">
+        <v>945</v>
+      </c>
+      <c r="I91" t="s">
+        <v>946</v>
+      </c>
+      <c r="J91" t="s">
+        <v>947</v>
+      </c>
+      <c r="K91" t="s">
+        <v>948</v>
+      </c>
+      <c r="L91" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>950</v>
+      </c>
+      <c r="D92" t="s">
+        <v>951</v>
+      </c>
+      <c r="E92" t="s">
+        <v>952</v>
+      </c>
+      <c r="F92" t="s">
+        <v>45</v>
+      </c>
+      <c r="G92" t="s">
+        <v>953</v>
+      </c>
+      <c r="H92" t="s">
+        <v>954</v>
+      </c>
+      <c r="I92" t="s">
+        <v>955</v>
+      </c>
+      <c r="J92" t="s">
+        <v>956</v>
+      </c>
+      <c r="K92" t="s">
+        <v>957</v>
+      </c>
+      <c r="L92" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>959</v>
+      </c>
+      <c r="D93" t="s">
+        <v>960</v>
+      </c>
+      <c r="E93" t="s">
+        <v>961</v>
+      </c>
+      <c r="F93" t="s">
+        <v>149</v>
+      </c>
+      <c r="G93" t="s">
+        <v>962</v>
+      </c>
+      <c r="H93" t="s">
+        <v>963</v>
+      </c>
+      <c r="I93" t="s">
+        <v>964</v>
+      </c>
+      <c r="J93" t="s">
+        <v>965</v>
+      </c>
+      <c r="K93" t="s">
+        <v>966</v>
+      </c>
+      <c r="L93" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>968</v>
+      </c>
+      <c r="D94" t="s">
+        <v>969</v>
+      </c>
+      <c r="E94" t="s">
+        <v>970</v>
+      </c>
+      <c r="F94" t="s">
+        <v>971</v>
+      </c>
+      <c r="G94" t="s">
+        <v>972</v>
+      </c>
+      <c r="H94" t="s">
+        <v>973</v>
+      </c>
+      <c r="I94" t="s">
+        <v>974</v>
+      </c>
+      <c r="J94" t="s">
+        <v>975</v>
+      </c>
+      <c r="K94" t="s">
+        <v>976</v>
+      </c>
+      <c r="L94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>977</v>
+      </c>
+      <c r="D95" t="s">
+        <v>978</v>
+      </c>
+      <c r="E95" t="s">
+        <v>979</v>
+      </c>
+      <c r="F95" t="s">
+        <v>980</v>
+      </c>
+      <c r="G95" t="s">
+        <v>981</v>
+      </c>
+      <c r="H95" t="s">
+        <v>982</v>
+      </c>
+      <c r="I95" t="s">
+        <v>983</v>
+      </c>
+      <c r="J95" t="s">
+        <v>984</v>
+      </c>
+      <c r="K95" t="s">
+        <v>100</v>
+      </c>
+      <c r="L95" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>986</v>
+      </c>
+      <c r="D96" t="s">
+        <v>658</v>
+      </c>
+      <c r="E96" t="s">
+        <v>987</v>
+      </c>
+      <c r="F96" t="s">
+        <v>988</v>
+      </c>
+      <c r="G96" t="s">
+        <v>918</v>
+      </c>
+      <c r="H96" t="s">
+        <v>989</v>
+      </c>
+      <c r="I96" t="s">
+        <v>990</v>
+      </c>
+      <c r="J96" t="s">
+        <v>991</v>
+      </c>
+      <c r="K96" t="s">
+        <v>992</v>
+      </c>
+      <c r="L96" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>994</v>
+      </c>
+      <c r="D97" t="s">
+        <v>737</v>
+      </c>
+      <c r="E97" t="s">
+        <v>995</v>
+      </c>
+      <c r="F97" t="s">
+        <v>996</v>
+      </c>
+      <c r="G97" t="s">
+        <v>997</v>
+      </c>
+      <c r="H97" t="s">
+        <v>998</v>
+      </c>
+      <c r="I97" t="s">
+        <v>999</v>
+      </c>
+      <c r="J97" t="s">
+        <v>1000</v>
+      </c>
+      <c r="K97" t="s">
+        <v>1001</v>
+      </c>
+      <c r="L97" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>103</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E98" t="s">
+        <v>547</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G98" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H98" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I98" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J98" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K98" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L98" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E99" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G99" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H99" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I99" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J99" t="s">
+        <v>1018</v>
+      </c>
+      <c r="K99" t="s">
+        <v>1019</v>
+      </c>
+      <c r="L99" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E100" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G100" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H100" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I100" t="s">
+        <v>1027</v>
+      </c>
+      <c r="J100" t="s">
+        <v>1028</v>
+      </c>
+      <c r="K100" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L100" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>106</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E101" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G101" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H101" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I101" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J101" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K101" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L101" t="s">
+        <v>1040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>